<commit_message>
modificações para atender demandas daniele, 16/09/2015
</commit_message>
<xml_diff>
--- a/Documentacao/03-Cronograma/ProductBacklog.xlsx
+++ b/Documentacao/03-Cronograma/ProductBacklog.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="7515" windowHeight="2325" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="7515" windowHeight="2325"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="4" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
     <sheet name="listagem" sheetId="6" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="92">
   <si>
     <t>Atividade</t>
   </si>
@@ -300,13 +300,30 @@
   <si>
     <t>controle câmera - acionar a câmera</t>
   </si>
+  <si>
+    <t>Previsão Finalizaçaõ</t>
+  </si>
+  <si>
+    <t>Ajustes eventuais</t>
+  </si>
+  <si>
+    <t>Monografia</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -358,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -373,11 +390,22 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -416,20 +444,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:K24" totalsRowShown="0">
-  <autoFilter ref="A2:K24"/>
-  <tableColumns count="11">
-    <tableColumn id="1" name="id" dataDxfId="8"/>
-    <tableColumn id="2" name="Sprint" dataDxfId="7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:L26" totalsRowShown="0">
+  <autoFilter ref="A2:L26"/>
+  <tableColumns count="12">
+    <tableColumn id="1" name="id" dataDxfId="9"/>
+    <tableColumn id="2" name="Sprint" dataDxfId="8"/>
     <tableColumn id="3" name="Atividade"/>
-    <tableColumn id="4" name="Responsável" dataDxfId="6"/>
-    <tableColumn id="5" name="Complexidade" dataDxfId="5"/>
-    <tableColumn id="6" name="Prioridade" dataDxfId="4"/>
-    <tableColumn id="7" name="Horas Estimadas" dataDxfId="3"/>
-    <tableColumn id="8" name="Horas realizadas" dataDxfId="2"/>
-    <tableColumn id="9" name="Status" dataDxfId="1"/>
-    <tableColumn id="11" name="% Percepção Finalização" dataDxfId="0"/>
+    <tableColumn id="4" name="Responsável" dataDxfId="7"/>
+    <tableColumn id="5" name="Complexidade" dataDxfId="6"/>
+    <tableColumn id="6" name="Prioridade" dataDxfId="5"/>
+    <tableColumn id="7" name="Horas Estimadas" dataDxfId="4"/>
+    <tableColumn id="8" name="Horas realizadas" dataDxfId="3"/>
+    <tableColumn id="9" name="Status" dataDxfId="2"/>
+    <tableColumn id="11" name="% Percepção Finalização" dataDxfId="1"/>
     <tableColumn id="10" name="Observações"/>
+    <tableColumn id="12" name="Previsão Finalizaçaõ" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -451,9 +480,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -491,7 +520,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -563,7 +592,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -737,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K24"/>
+  <dimension ref="A2:L30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,9 +784,10 @@
     <col min="9" max="9" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="46.140625" customWidth="1"/>
+    <col min="12" max="12" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>36</v>
       </c>
@@ -791,8 +821,11 @@
       <c r="K2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -826,8 +859,11 @@
       <c r="K3" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="9">
+        <v>41796</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -858,8 +894,11 @@
       <c r="J4" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="9">
+        <v>42272</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -890,8 +929,11 @@
       <c r="J5" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="9">
+        <v>42272</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -922,8 +964,11 @@
       <c r="J6" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="9">
+        <v>42272</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -957,8 +1002,11 @@
       <c r="K7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="9">
+        <v>42272</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -986,8 +1034,11 @@
       <c r="I8" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="9">
+        <v>42272</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -1015,8 +1066,11 @@
       <c r="I9" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="9">
+        <v>42272</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1047,8 +1101,11 @@
       <c r="K10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="9">
+        <v>42272</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1076,8 +1133,11 @@
       <c r="I11" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="9">
+        <v>42272</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1105,8 +1165,11 @@
       <c r="I12" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="9">
+        <v>42279</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1134,8 +1197,11 @@
       <c r="I13" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="9">
+        <v>42279</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1163,8 +1229,11 @@
       <c r="I14" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="9">
+        <v>42279</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -1192,8 +1261,11 @@
       <c r="I15" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="9">
+        <v>42279</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -1221,8 +1293,11 @@
       <c r="I16" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L16" s="9">
+        <v>42279</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -1250,8 +1325,11 @@
       <c r="I17" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L17" s="9">
+        <v>42279</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -1279,8 +1357,11 @@
       <c r="I18" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L18" s="9">
+        <v>42279</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -1308,8 +1389,11 @@
       <c r="I19" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L19" s="9">
+        <v>42286</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -1337,8 +1421,11 @@
       <c r="I20" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L20" s="9">
+        <v>42286</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -1366,8 +1453,11 @@
       <c r="I21" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L21" s="9">
+        <v>42286</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -1395,8 +1485,11 @@
       <c r="I22" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L22" s="10">
+        <v>42286</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -1424,8 +1517,11 @@
       <c r="I23" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="L23" s="10">
+        <v>42286</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -1453,6 +1549,73 @@
       <c r="I24" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="L24" s="10">
+        <v>42293</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="2">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="2">
+        <v>4</v>
+      </c>
+      <c r="F25" s="2">
+        <v>9</v>
+      </c>
+      <c r="G25" s="2">
+        <v>16</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L25" s="10">
+        <v>42293</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="2">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="2">
+        <v>9</v>
+      </c>
+      <c r="F26" s="2">
+        <v>9</v>
+      </c>
+      <c r="G26" s="2">
+        <v>80</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L26" s="10">
+        <v>42300</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K29" s="11"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K30" s="8"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
@@ -1491,7 +1654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>

</xml_diff>